<commit_message>
DIR 18/04: Data Center terminado
Falta hacer comprobaciones con simulación.
</commit_message>
<xml_diff>
--- a/DIR/Proyecto/P1-e5 Data Center/GIC-DIR-Práctica1-e5/GIC-DIR-Practica2-e2-VLANs_v5.xlsx
+++ b/DIR/Proyecto/P1-e5 Data Center/GIC-DIR-Práctica1-e5/GIC-DIR-Practica2-e2-VLANs_v5.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="108">
   <si>
     <t>Depts.</t>
   </si>
@@ -180,9 +180,6 @@
     <t>10.1.2.0/23</t>
   </si>
   <si>
-    <t>10.1.2.1</t>
-  </si>
-  <si>
     <t>APP1-L2DB</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
     <t>10.1.4.0/23</t>
   </si>
   <si>
-    <t>10.1.4.1</t>
-  </si>
-  <si>
     <t>APP2-Front</t>
   </si>
   <si>
@@ -216,9 +210,6 @@
     <t>10.1.8.0/23</t>
   </si>
   <si>
-    <t>10.1.8.1</t>
-  </si>
-  <si>
     <t>APP2-L2DB</t>
   </si>
   <si>
@@ -226,9 +217,6 @@
   </si>
   <si>
     <t>10.1.10.0/23</t>
-  </si>
-  <si>
-    <t>10.1.10.1</t>
   </si>
   <si>
     <t>DNS</t>
@@ -1020,6 +1008,30 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1047,33 +1059,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="32" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1117,7 +1105,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{56181EE2-1A24-2739-B7C7-DDB8F2EB4828}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56181EE2-1A24-2739-B7C7-DDB8F2EB4828}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1435,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU54"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="123" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:H54"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="123" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,11 +1767,11 @@
       </c>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="55"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="69"/>
       <c r="J12" s="22">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -1894,11 +1882,11 @@
       </c>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
+      <c r="A13" s="70" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="58"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="72"/>
       <c r="J13" s="22">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -1913,11 +1901,11 @@
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="70" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="58"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="72"/>
       <c r="J14" s="22">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -1939,11 +1927,11 @@
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
+      <c r="A15" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="60"/>
-      <c r="C15" s="61"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="75"/>
       <c r="J15" s="22">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -2063,17 +2051,15 @@
       <c r="F26" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="34" t="s">
-        <v>49</v>
-      </c>
+      <c r="G26" s="34"/>
       <c r="H26" s="42"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="34" t="s">
         <v>50</v>
-      </c>
-      <c r="B27" s="34" t="s">
-        <v>51</v>
       </c>
       <c r="C27" s="34"/>
       <c r="D27" s="34">
@@ -2083,19 +2069,17 @@
         <v>512</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="34" t="s">
-        <v>53</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="G27" s="34"/>
       <c r="H27" s="42"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C28" s="34"/>
       <c r="D28" s="34">
@@ -2105,19 +2089,19 @@
         <v>512</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H28" s="44"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" s="34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" s="34"/>
       <c r="D29" s="34">
@@ -2127,19 +2111,17 @@
         <v>512</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29" s="34" t="s">
-        <v>61</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="G29" s="34"/>
       <c r="H29" s="42"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B30" s="34" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C30" s="34"/>
       <c r="D30" s="34">
@@ -2149,19 +2131,17 @@
         <v>512</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="G30" s="34" t="s">
-        <v>65</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G30" s="34"/>
       <c r="H30" s="42"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="43" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C31" s="36"/>
       <c r="D31" s="36">
@@ -2171,10 +2151,10 @@
         <v>512</v>
       </c>
       <c r="F31" s="36" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="G31" s="36" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H31" s="42"/>
     </row>
@@ -2203,25 +2183,25 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C38" s="39" t="s">
         <v>2</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E38" s="39" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F38" s="39" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G38" s="39" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H38" s="40" t="s">
         <v>7</v>
@@ -2229,7 +2209,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="41" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B39" s="34">
         <v>0</v>
@@ -2239,19 +2219,19 @@
       </c>
       <c r="D39" s="34"/>
       <c r="E39" s="34" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F39" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H39" s="42"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="41" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B40" s="34">
         <v>0</v>
@@ -2261,19 +2241,19 @@
       </c>
       <c r="D40" s="34"/>
       <c r="E40" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F40" s="34" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H40" s="42"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B41" s="34">
         <v>0</v>
@@ -2283,7 +2263,7 @@
       </c>
       <c r="D41" s="34"/>
       <c r="E41" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F41" s="35"/>
       <c r="G41" s="35"/>
@@ -2291,7 +2271,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="43" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B42" s="34">
         <v>0</v>
@@ -2301,7 +2281,7 @@
       </c>
       <c r="D42" s="34"/>
       <c r="E42" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F42" s="35"/>
       <c r="G42" s="35"/>
@@ -2309,7 +2289,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="41" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B43" s="34">
         <v>1</v>
@@ -2319,7 +2299,7 @@
       </c>
       <c r="D43" s="34"/>
       <c r="E43" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F43" s="35"/>
       <c r="G43" s="35"/>
@@ -2327,7 +2307,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="41" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B44" s="34">
         <v>1</v>
@@ -2337,7 +2317,7 @@
       </c>
       <c r="D44" s="34"/>
       <c r="E44" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F44" s="35"/>
       <c r="G44" s="35"/>
@@ -2345,7 +2325,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="43" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B45" s="36">
         <v>2</v>
@@ -2355,7 +2335,7 @@
       </c>
       <c r="D45" s="36"/>
       <c r="E45" s="36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F45" s="36"/>
       <c r="G45" s="36"/>
@@ -2363,7 +2343,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="41" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B46" s="34">
         <v>2</v>
@@ -2373,7 +2353,7 @@
       </c>
       <c r="D46" s="34"/>
       <c r="E46" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F46" s="35"/>
       <c r="G46" s="35"/>
@@ -2381,7 +2361,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B47" s="34">
         <v>0</v>
@@ -2391,7 +2371,7 @@
       </c>
       <c r="D47" s="34"/>
       <c r="E47" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F47" s="35"/>
       <c r="G47" s="35"/>
@@ -2399,7 +2379,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="43" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B48" s="37">
         <v>0</v>
@@ -2409,7 +2389,7 @@
       </c>
       <c r="D48" s="36"/>
       <c r="E48" s="36" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F48" s="36"/>
       <c r="G48" s="36"/>
@@ -2417,7 +2397,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="41" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B49" s="34">
         <v>0</v>
@@ -2427,7 +2407,7 @@
       </c>
       <c r="D49" s="34"/>
       <c r="E49" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F49" s="35"/>
       <c r="G49" s="35"/>
@@ -2435,7 +2415,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B50" s="34">
         <v>0</v>
@@ -2445,7 +2425,7 @@
       </c>
       <c r="D50" s="34"/>
       <c r="E50" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F50" s="35"/>
       <c r="G50" s="35"/>
@@ -2453,7 +2433,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="41" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B51" s="34">
         <v>0</v>
@@ -2463,7 +2443,7 @@
       </c>
       <c r="D51" s="34"/>
       <c r="E51" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F51" s="35"/>
       <c r="G51" s="35"/>
@@ -2471,7 +2451,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="41" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B52" s="34">
         <v>0</v>
@@ -2481,7 +2461,7 @@
       </c>
       <c r="D52" s="34"/>
       <c r="E52" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F52" s="35"/>
       <c r="G52" s="35"/>
@@ -2489,7 +2469,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="41" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B53" s="34">
         <v>0</v>
@@ -2499,7 +2479,7 @@
       </c>
       <c r="D53" s="34"/>
       <c r="E53" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F53" s="35"/>
       <c r="G53" s="35"/>
@@ -2507,7 +2487,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="41" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B54" s="34">
         <v>0</v>
@@ -2517,7 +2497,7 @@
       </c>
       <c r="D54" s="34"/>
       <c r="E54" s="34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F54" s="35"/>
       <c r="G54" s="35"/>
@@ -2543,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:R28"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2556,53 +2536,53 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
+      <c r="A3" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="76"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
     </row>
     <row r="4" spans="1:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
-        <v>100</v>
-      </c>
-      <c r="B4" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="72" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="72" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="74"/>
-      <c r="K4" s="76"/>
-      <c r="L4" s="76"/>
-      <c r="M4" s="76"/>
-      <c r="N4" s="76"/>
-      <c r="O4" s="76"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="76"/>
+      <c r="A4" s="62" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="65"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -2611,21 +2591,21 @@
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
       <c r="I5" s="42"/>
-      <c r="K5" s="76"/>
-      <c r="L5" s="76"/>
-      <c r="M5" s="76"/>
-      <c r="N5" s="76"/>
-      <c r="O5" s="76"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="76"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
@@ -2634,21 +2614,21 @@
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
       <c r="I6" s="42"/>
-      <c r="K6" s="76"/>
-      <c r="L6" s="76"/>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
-      <c r="R6" s="76"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="66"/>
+      <c r="O6" s="66"/>
+      <c r="P6" s="66"/>
+      <c r="Q6" s="66"/>
+      <c r="R6" s="66"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
@@ -2657,18 +2637,18 @@
       <c r="G7" s="35"/>
       <c r="H7" s="35"/>
       <c r="I7" s="42"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="76"/>
-      <c r="N7" s="76"/>
-      <c r="O7" s="76"/>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
-      <c r="R7" s="76"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="66"/>
+      <c r="O7" s="66"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="66"/>
+      <c r="R7" s="66"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="41" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B8" s="35"/>
       <c r="C8" s="34"/>
@@ -2678,18 +2658,18 @@
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
       <c r="I8" s="44"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
-      <c r="N8" s="76"/>
-      <c r="O8" s="76"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
-      <c r="R8" s="76"/>
+      <c r="K8" s="66"/>
+      <c r="L8" s="66"/>
+      <c r="M8" s="66"/>
+      <c r="N8" s="66"/>
+      <c r="O8" s="66"/>
+      <c r="P8" s="66"/>
+      <c r="Q8" s="66"/>
+      <c r="R8" s="66"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="41" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B9" s="34"/>
       <c r="C9" s="34"/>
@@ -2699,18 +2679,18 @@
       <c r="G9" s="35"/>
       <c r="H9" s="35"/>
       <c r="I9" s="42"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="76"/>
-      <c r="M9" s="76"/>
-      <c r="N9" s="76"/>
-      <c r="O9" s="76"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="76"/>
+      <c r="K9" s="66"/>
+      <c r="L9" s="66"/>
+      <c r="M9" s="66"/>
+      <c r="N9" s="66"/>
+      <c r="O9" s="66"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
+      <c r="R9" s="66"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="41" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B10" s="34"/>
       <c r="C10" s="34"/>
@@ -2720,18 +2700,18 @@
       <c r="G10" s="35"/>
       <c r="H10" s="35"/>
       <c r="I10" s="42"/>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
-      <c r="N10" s="76"/>
-      <c r="O10" s="76"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="76"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B11" s="36"/>
       <c r="C11" s="36"/>
@@ -2741,21 +2721,21 @@
       <c r="G11" s="36"/>
       <c r="H11" s="36"/>
       <c r="I11" s="42"/>
-      <c r="K11" s="76"/>
-      <c r="L11" s="76"/>
-      <c r="M11" s="76"/>
-      <c r="N11" s="76"/>
-      <c r="O11" s="76"/>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="76"/>
-      <c r="R11" s="76"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="41" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -2764,134 +2744,134 @@
       <c r="G12" s="35"/>
       <c r="H12" s="35"/>
       <c r="I12" s="42"/>
-      <c r="K12" s="76"/>
-      <c r="L12" s="76"/>
-      <c r="M12" s="76"/>
-      <c r="N12" s="76"/>
-      <c r="O12" s="76"/>
-      <c r="P12" s="76"/>
-      <c r="Q12" s="76"/>
-      <c r="R12" s="76"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="62" t="s">
-        <v>84</v>
-      </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="67"/>
-      <c r="I13" s="63"/>
-      <c r="K13" s="76"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="76"/>
-      <c r="N13" s="76"/>
-      <c r="O13" s="76"/>
-      <c r="P13" s="76"/>
-      <c r="Q13" s="76"/>
-      <c r="R13" s="76"/>
+        <v>105</v>
+      </c>
+      <c r="B13" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="53"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="54"/>
+      <c r="K13" s="66"/>
+      <c r="L13" s="66"/>
+      <c r="M13" s="66"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="66"/>
+      <c r="P13" s="66"/>
+      <c r="Q13" s="66"/>
+      <c r="R13" s="66"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="C14" s="70"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="76"/>
-      <c r="N14" s="76"/>
-      <c r="O14" s="76"/>
-      <c r="P14" s="76"/>
-      <c r="Q14" s="76"/>
-      <c r="R14" s="76"/>
+        <v>106</v>
+      </c>
+      <c r="B14" s="61" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="61"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="66"/>
+      <c r="P14" s="66"/>
+      <c r="Q14" s="66"/>
+      <c r="R14" s="66"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="65"/>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="66"/>
-      <c r="H15" s="66"/>
-      <c r="I15" s="65"/>
-      <c r="K15" s="76"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="76"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="76"/>
-      <c r="R15" s="76"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="56"/>
+      <c r="K15" s="66"/>
+      <c r="L15" s="66"/>
+      <c r="M15" s="66"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="66"/>
+      <c r="P15" s="66"/>
+      <c r="Q15" s="66"/>
+      <c r="R15" s="66"/>
     </row>
     <row r="16" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="75" t="s">
-        <v>80</v>
-      </c>
-      <c r="B16" s="75"/>
-      <c r="C16" s="75"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="75"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="76"/>
-      <c r="N16" s="76"/>
-      <c r="O16" s="76"/>
-      <c r="P16" s="76"/>
-      <c r="Q16" s="76"/>
-      <c r="R16" s="76"/>
+      <c r="A16" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="K16" s="66"/>
+      <c r="L16" s="66"/>
+      <c r="M16" s="66"/>
+      <c r="N16" s="66"/>
+      <c r="O16" s="66"/>
+      <c r="P16" s="66"/>
+      <c r="Q16" s="66"/>
+      <c r="R16" s="66"/>
     </row>
     <row r="17" spans="1:18" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="B17" s="72" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="72" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="73"/>
-      <c r="G17" s="73"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="74"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
+      <c r="A17" s="62" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="E17" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="64"/>
+      <c r="G17" s="64"/>
+      <c r="H17" s="64"/>
+      <c r="I17" s="65"/>
+      <c r="K17" s="66"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="66"/>
+      <c r="P17" s="66"/>
+      <c r="Q17" s="66"/>
+      <c r="R17" s="66"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="41" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="34"/>
@@ -2900,21 +2880,21 @@
       <c r="G18" s="34"/>
       <c r="H18" s="34"/>
       <c r="I18" s="42"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
-      <c r="P18" s="76"/>
-      <c r="Q18" s="76"/>
-      <c r="R18" s="76"/>
+      <c r="K18" s="66"/>
+      <c r="L18" s="66"/>
+      <c r="M18" s="66"/>
+      <c r="N18" s="66"/>
+      <c r="O18" s="66"/>
+      <c r="P18" s="66"/>
+      <c r="Q18" s="66"/>
+      <c r="R18" s="66"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="41" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C19" s="34"/>
       <c r="D19" s="34"/>
@@ -2923,18 +2903,18 @@
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
       <c r="I19" s="42"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="76"/>
-      <c r="N19" s="76"/>
-      <c r="O19" s="76"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="76"/>
+      <c r="K19" s="66"/>
+      <c r="L19" s="66"/>
+      <c r="M19" s="66"/>
+      <c r="N19" s="66"/>
+      <c r="O19" s="66"/>
+      <c r="P19" s="66"/>
+      <c r="Q19" s="66"/>
+      <c r="R19" s="66"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B20" s="34"/>
       <c r="C20" s="34"/>
@@ -2944,18 +2924,18 @@
       <c r="G20" s="35"/>
       <c r="H20" s="35"/>
       <c r="I20" s="42"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="76"/>
-      <c r="N20" s="76"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="76"/>
-      <c r="Q20" s="76"/>
-      <c r="R20" s="76"/>
+      <c r="K20" s="66"/>
+      <c r="L20" s="66"/>
+      <c r="M20" s="66"/>
+      <c r="N20" s="66"/>
+      <c r="O20" s="66"/>
+      <c r="P20" s="66"/>
+      <c r="Q20" s="66"/>
+      <c r="R20" s="66"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="41" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B21" s="34"/>
       <c r="C21" s="34"/>
@@ -2965,18 +2945,18 @@
       <c r="G21" s="35"/>
       <c r="H21" s="35"/>
       <c r="I21" s="44"/>
-      <c r="K21" s="76"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="76"/>
-      <c r="N21" s="76"/>
-      <c r="O21" s="76"/>
-      <c r="P21" s="76"/>
-      <c r="Q21" s="76"/>
-      <c r="R21" s="76"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="66"/>
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="66"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="41" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
@@ -2986,18 +2966,18 @@
       <c r="G22" s="35"/>
       <c r="H22" s="35"/>
       <c r="I22" s="42"/>
-      <c r="K22" s="76"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="76"/>
-      <c r="N22" s="76"/>
-      <c r="O22" s="76"/>
-      <c r="P22" s="76"/>
-      <c r="Q22" s="76"/>
-      <c r="R22" s="76"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B23" s="34"/>
       <c r="C23" s="34"/>
@@ -3007,18 +2987,18 @@
       <c r="G23" s="35"/>
       <c r="H23" s="35"/>
       <c r="I23" s="42"/>
-      <c r="K23" s="76"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="76"/>
-      <c r="N23" s="76"/>
-      <c r="O23" s="76"/>
-      <c r="P23" s="76"/>
-      <c r="Q23" s="76"/>
-      <c r="R23" s="76"/>
+      <c r="K23" s="66"/>
+      <c r="L23" s="66"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="66"/>
+      <c r="O23" s="66"/>
+      <c r="P23" s="66"/>
+      <c r="Q23" s="66"/>
+      <c r="R23" s="66"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="41" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -3028,21 +3008,21 @@
       <c r="G24" s="36"/>
       <c r="H24" s="36"/>
       <c r="I24" s="42"/>
-      <c r="K24" s="76"/>
-      <c r="L24" s="76"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="76"/>
-      <c r="O24" s="76"/>
-      <c r="P24" s="76"/>
-      <c r="Q24" s="76"/>
-      <c r="R24" s="76"/>
+      <c r="K24" s="66"/>
+      <c r="L24" s="66"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="66"/>
+      <c r="O24" s="66"/>
+      <c r="P24" s="66"/>
+      <c r="Q24" s="66"/>
+      <c r="R24" s="66"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="41" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B25" s="34" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C25" s="34"/>
       <c r="D25" s="34"/>
@@ -3051,70 +3031,70 @@
       <c r="G25" s="35"/>
       <c r="H25" s="35"/>
       <c r="I25" s="42"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="76"/>
-      <c r="N25" s="76"/>
-      <c r="O25" s="76"/>
-      <c r="P25" s="76"/>
-      <c r="Q25" s="76"/>
-      <c r="R25" s="76"/>
+      <c r="K25" s="66"/>
+      <c r="L25" s="66"/>
+      <c r="M25" s="66"/>
+      <c r="N25" s="66"/>
+      <c r="O25" s="66"/>
+      <c r="P25" s="66"/>
+      <c r="Q25" s="66"/>
+      <c r="R25" s="66"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="41" t="s">
-        <v>109</v>
-      </c>
-      <c r="B26" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="63"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="76"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="76"/>
-      <c r="O26" s="76"/>
-      <c r="P26" s="76"/>
-      <c r="Q26" s="76"/>
-      <c r="R26" s="76"/>
+        <v>105</v>
+      </c>
+      <c r="B26" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="53"/>
+      <c r="F26" s="53"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="54"/>
+      <c r="K26" s="66"/>
+      <c r="L26" s="66"/>
+      <c r="M26" s="66"/>
+      <c r="N26" s="66"/>
+      <c r="O26" s="66"/>
+      <c r="P26" s="66"/>
+      <c r="Q26" s="66"/>
+      <c r="R26" s="66"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="B27" s="70" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="70"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="76"/>
-      <c r="N27" s="76"/>
-      <c r="O27" s="76"/>
-      <c r="P27" s="76"/>
-      <c r="Q27" s="76"/>
-      <c r="R27" s="76"/>
+        <v>106</v>
+      </c>
+      <c r="B27" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27" s="61"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="66"/>
+      <c r="M27" s="66"/>
+      <c r="N27" s="66"/>
+      <c r="O27" s="66"/>
+      <c r="P27" s="66"/>
+      <c r="Q27" s="66"/>
+      <c r="R27" s="66"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K28" s="76"/>
-      <c r="L28" s="76"/>
-      <c r="M28" s="76"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="76"/>
-      <c r="P28" s="76"/>
-      <c r="Q28" s="76"/>
-      <c r="R28" s="76"/>
+      <c r="K28" s="66"/>
+      <c r="L28" s="66"/>
+      <c r="M28" s="66"/>
+      <c r="N28" s="66"/>
+      <c r="O28" s="66"/>
+      <c r="P28" s="66"/>
+      <c r="Q28" s="66"/>
+      <c r="R28" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>